<commit_message>
Edited graph a bit
</commit_message>
<xml_diff>
--- a/StepSizeData.xlsx
+++ b/StepSizeData.xlsx
@@ -1054,8 +1054,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Cumulative Reward</a:t>
+                  <a:t>Completion</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -26962,12 +26967,12 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>

</xml_diff>